<commit_message>
initial slides to Glen
</commit_message>
<xml_diff>
--- a/munroe-francis_duplicates.xlsx
+++ b/munroe-francis_duplicates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephen-krewson\Documents\project-hathi-images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13139F79-75BE-4B46-9B3B-C659159FE77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACDD47A-7B7B-46CD-A5E8-8C97EE574137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{0DC18770-C6C2-42EC-906F-B2E44E51572D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0DC18770-C6C2-42EC-906F-B2E44E51572D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>